<commit_message>
report delta distribution among edges
</commit_message>
<xml_diff>
--- a/experiment_observation_time.xlsx
+++ b/experiment_observation_time.xlsx
@@ -8,20 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Gamal Elkoumy\PhD\OneDrive - Tartu Ülikool\Differential Privacy\source code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F9F8140-F8B5-429A-8100-4753B07717B0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D3AA3ED-B4D7-425B-B848-AF62F783DB9D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{76BF992B-08E0-4334-A30A-99A6967A2729}"/>
   </bookViews>
   <sheets>
     <sheet name="delta-dashboard" sheetId="3" r:id="rId1"/>
     <sheet name="delta-input" sheetId="1" r:id="rId2"/>
-    <sheet name="alpha-dashboard" sheetId="4" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="5" r:id="rId3"/>
     <sheet name="alpha-input" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <pivotCaches>
-    <pivotCache cacheId="18" r:id="rId5"/>
-    <pivotCache cacheId="23" r:id="rId6"/>
+    <pivotCache cacheId="0" r:id="rId5"/>
+    <pivotCache cacheId="6" r:id="rId6"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="24">
   <si>
     <t>dataset</t>
   </si>
@@ -213,7 +213,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Gamal Elkomy" refreshedDate="44056.539800694445" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="43" xr:uid="{6A17816E-9251-45D8-9E36-7CAB4055D11F}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Gamal Elkomy" refreshedDate="44056.705103356479" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="49" xr:uid="{9534F982-D5A9-4617-A98C-7ACE13BBEB49}">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:F1048576" sheet="alpha-input"/>
   </cacheSource>
@@ -237,22 +237,23 @@
       <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="0" maxValue="0"/>
     </cacheField>
     <cacheField name="alpha" numFmtId="0">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="10" maxValue="10000" count="8">
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="0.1" maxValue="20" count="9">
+        <n v="0.1"/>
+        <n v="0.3"/>
+        <n v="0.5"/>
+        <n v="0.7"/>
+        <n v="1"/>
+        <n v="2"/>
         <n v="10"/>
-        <n v="50"/>
-        <n v="100"/>
-        <n v="500"/>
-        <n v="1000"/>
-        <n v="5000"/>
-        <n v="10000"/>
+        <n v="20"/>
         <m/>
       </sharedItems>
     </cacheField>
     <cacheField name="epsilon_time" numFmtId="0">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="2.9957322735539902E-4" maxValue="0.29957322735539899"/>
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="0.14978661367769899" maxValue="29.957322735539901"/>
     </cacheField>
     <cacheField name="delta_time" numFmtId="0">
-      <sharedItems containsBlank="1" containsMixedTypes="1" containsNumber="1" minValue="0.99765258215962405" maxValue="0.99943757030371205"/>
+      <sharedItems containsBlank="1" containsMixedTypes="1" containsNumber="1" minValue="0.99756097560975598" maxValue="0.99943757030371205"/>
     </cacheField>
   </cacheFields>
   <extLst>
@@ -469,12 +470,60 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="43">
-  <r>
-    <x v="0"/>
-    <x v="0"/>
-    <n v="0"/>
-    <x v="0"/>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="49">
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="0"/>
+    <x v="0"/>
+    <n v="29.957322735539901"/>
+    <s v="[]"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="0"/>
+    <x v="1"/>
+    <n v="9.9857742451799698"/>
+    <s v="[]"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="0"/>
+    <x v="2"/>
+    <n v="5.9914645471079799"/>
+    <s v="[]"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="0"/>
+    <x v="3"/>
+    <n v="4.2796175336485502"/>
+    <s v="[]"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="0"/>
+    <x v="4"/>
+    <n v="2.99573227355399"/>
+    <s v="[]"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="0"/>
+    <x v="5"/>
+    <n v="1.4978661367769901"/>
+    <s v="[]"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="0"/>
+    <x v="6"/>
     <n v="0.29957322735539899"/>
     <s v="[]"/>
   </r>
@@ -482,55 +531,63 @@
     <x v="0"/>
     <x v="0"/>
     <n v="0"/>
-    <x v="1"/>
-    <n v="5.9914645471079803E-2"/>
+    <x v="7"/>
+    <n v="0.14978661367769899"/>
     <s v="[]"/>
   </r>
   <r>
     <x v="0"/>
-    <x v="0"/>
-    <n v="0"/>
-    <x v="2"/>
-    <n v="2.9957322735539901E-2"/>
+    <x v="1"/>
+    <n v="0"/>
+    <x v="0"/>
+    <n v="29.957322735539901"/>
     <s v="[]"/>
   </r>
   <r>
     <x v="0"/>
-    <x v="0"/>
+    <x v="1"/>
+    <n v="0"/>
+    <x v="1"/>
+    <n v="9.9857742451799698"/>
+    <s v="[]"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="0"/>
+    <x v="2"/>
+    <n v="5.9914645471079799"/>
+    <s v="[]"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="1"/>
     <n v="0"/>
     <x v="3"/>
-    <n v="5.9914645471079797E-3"/>
+    <n v="4.2796175336485502"/>
     <s v="[]"/>
   </r>
   <r>
     <x v="0"/>
-    <x v="0"/>
+    <x v="1"/>
     <n v="0"/>
     <x v="4"/>
-    <n v="2.9957322735539899E-3"/>
+    <n v="2.99573227355399"/>
     <s v="[]"/>
   </r>
   <r>
     <x v="0"/>
-    <x v="0"/>
+    <x v="1"/>
     <n v="0"/>
     <x v="5"/>
-    <n v="5.9914645471079804E-4"/>
+    <n v="1.4978661367769901"/>
     <s v="[]"/>
   </r>
   <r>
     <x v="0"/>
-    <x v="0"/>
+    <x v="1"/>
     <n v="0"/>
     <x v="6"/>
-    <n v="2.9957322735539902E-4"/>
-    <s v="[]"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="1"/>
-    <n v="0"/>
-    <x v="0"/>
     <n v="0.29957322735539899"/>
     <s v="[]"/>
   </r>
@@ -538,55 +595,63 @@
     <x v="0"/>
     <x v="1"/>
     <n v="0"/>
-    <x v="1"/>
-    <n v="5.9914645471079803E-2"/>
+    <x v="7"/>
+    <n v="0.14978661367769899"/>
     <s v="[]"/>
   </r>
   <r>
-    <x v="0"/>
-    <x v="1"/>
-    <n v="0"/>
-    <x v="2"/>
-    <n v="2.9957322735539901E-2"/>
-    <s v="[]"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="1"/>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="0"/>
+    <x v="0"/>
+    <n v="29.957322735539901"/>
+    <n v="0.99943757030371205"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="0"/>
+    <x v="1"/>
+    <n v="9.9857742451799698"/>
+    <n v="0.99943757030371205"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="0"/>
+    <x v="2"/>
+    <n v="5.9914645471079799"/>
+    <n v="0.99943757030371205"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="0"/>
     <n v="0"/>
     <x v="3"/>
-    <n v="5.9914645471079797E-3"/>
-    <s v="[]"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="1"/>
+    <n v="4.2796175336485502"/>
+    <n v="0.99943757030371205"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="0"/>
     <n v="0"/>
     <x v="4"/>
-    <n v="2.9957322735539899E-3"/>
-    <s v="[]"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="1"/>
+    <n v="2.99573227355399"/>
+    <n v="0.99943757030371205"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="0"/>
     <n v="0"/>
     <x v="5"/>
-    <n v="5.9914645471079804E-4"/>
-    <s v="[]"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="1"/>
+    <n v="1.4978661367769901"/>
+    <n v="0.99943757030371205"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="0"/>
     <n v="0"/>
     <x v="6"/>
-    <n v="2.9957322735539902E-4"/>
-    <s v="[]"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="0"/>
-    <n v="0"/>
-    <x v="0"/>
     <n v="0.29957322735539899"/>
     <n v="0.99943757030371205"/>
   </r>
@@ -594,55 +659,63 @@
     <x v="1"/>
     <x v="0"/>
     <n v="0"/>
-    <x v="1"/>
-    <n v="5.9914645471079803E-2"/>
+    <x v="7"/>
+    <n v="0.14978661367769899"/>
+    <n v="0.99943757030343505"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="0"/>
+    <x v="0"/>
+    <n v="29.957322735539901"/>
     <n v="0.99943757030371205"/>
   </r>
   <r>
     <x v="1"/>
-    <x v="0"/>
-    <n v="0"/>
-    <x v="2"/>
-    <n v="2.9957322735539901E-2"/>
+    <x v="1"/>
+    <n v="0"/>
+    <x v="1"/>
+    <n v="9.9857742451799698"/>
     <n v="0.99943757030371205"/>
   </r>
   <r>
     <x v="1"/>
-    <x v="0"/>
+    <x v="1"/>
+    <n v="0"/>
+    <x v="2"/>
+    <n v="5.9914645471079799"/>
+    <n v="0.99943757030371205"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="1"/>
     <n v="0"/>
     <x v="3"/>
-    <n v="5.9914645471079797E-3"/>
+    <n v="4.2796175336485502"/>
     <n v="0.99943757030371205"/>
   </r>
   <r>
     <x v="1"/>
-    <x v="0"/>
+    <x v="1"/>
     <n v="0"/>
     <x v="4"/>
-    <n v="2.9957322735539899E-3"/>
+    <n v="2.99573227355399"/>
     <n v="0.99943757030371205"/>
   </r>
   <r>
     <x v="1"/>
-    <x v="0"/>
+    <x v="1"/>
     <n v="0"/>
     <x v="5"/>
-    <n v="5.9914645471079804E-4"/>
+    <n v="1.4978661367769901"/>
     <n v="0.99943757030371205"/>
   </r>
   <r>
     <x v="1"/>
-    <x v="0"/>
+    <x v="1"/>
     <n v="0"/>
     <x v="6"/>
-    <n v="2.9957322735539902E-4"/>
-    <n v="0.99943757030371205"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="1"/>
-    <n v="0"/>
-    <x v="0"/>
     <n v="0.29957322735539899"/>
     <n v="0.99943757030371205"/>
   </r>
@@ -650,167 +723,143 @@
     <x v="1"/>
     <x v="1"/>
     <n v="0"/>
-    <x v="1"/>
-    <n v="5.9914645471079803E-2"/>
-    <n v="0.99943757030371205"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="1"/>
-    <n v="0"/>
-    <x v="2"/>
-    <n v="2.9957322735539901E-2"/>
-    <n v="0.99943757030371205"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="1"/>
+    <x v="7"/>
+    <n v="0.14978661367769899"/>
+    <n v="0.99943757030343505"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="0"/>
+    <n v="0"/>
+    <x v="0"/>
+    <n v="29.957322735539901"/>
+    <n v="0.99756097560975598"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="0"/>
+    <n v="0"/>
+    <x v="1"/>
+    <n v="9.9857742451799698"/>
+    <n v="0.99756097560975598"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="0"/>
+    <n v="0"/>
+    <x v="2"/>
+    <n v="5.9914645471079799"/>
+    <n v="0.99756097560975598"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="0"/>
     <n v="0"/>
     <x v="3"/>
-    <n v="5.9914645471079797E-3"/>
-    <n v="0.99943757030371205"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="1"/>
+    <n v="4.2796175336485502"/>
+    <n v="0.99756097560975598"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="0"/>
     <n v="0"/>
     <x v="4"/>
-    <n v="2.9957322735539899E-3"/>
-    <n v="0.99943757030371205"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="1"/>
+    <n v="2.99573227355399"/>
+    <n v="0.99756097560975598"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="0"/>
     <n v="0"/>
     <x v="5"/>
-    <n v="5.9914645471079804E-4"/>
-    <n v="0.99943757030371205"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="1"/>
+    <n v="1.4978661367769901"/>
+    <n v="0.99756097560975598"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="0"/>
     <n v="0"/>
     <x v="6"/>
-    <n v="2.9957322735539902E-4"/>
-    <n v="0.99943757030371205"/>
-  </r>
-  <r>
-    <x v="2"/>
-    <x v="0"/>
-    <n v="0"/>
-    <x v="0"/>
     <n v="0.29957322735539899"/>
-    <n v="0.99765258215962405"/>
-  </r>
-  <r>
-    <x v="2"/>
-    <x v="0"/>
-    <n v="0"/>
-    <x v="1"/>
-    <n v="5.9914645471079803E-2"/>
-    <n v="0.99765258215962405"/>
-  </r>
-  <r>
-    <x v="2"/>
-    <x v="0"/>
-    <n v="0"/>
-    <x v="2"/>
-    <n v="2.9957322735539901E-2"/>
-    <n v="0.99765258215962405"/>
-  </r>
-  <r>
-    <x v="2"/>
-    <x v="0"/>
+    <n v="0.99756097560975598"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="0"/>
+    <n v="0"/>
+    <x v="7"/>
+    <n v="0.14978661367769899"/>
+    <n v="0.99756097560975598"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="0"/>
+    <x v="0"/>
+    <n v="29.957322735539901"/>
+    <n v="0.99756097560975598"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="0"/>
+    <x v="1"/>
+    <n v="9.9857742451799698"/>
+    <n v="0.99756097560975598"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="0"/>
+    <x v="2"/>
+    <n v="5.9914645471079799"/>
+    <n v="0.99756097560975598"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="1"/>
     <n v="0"/>
     <x v="3"/>
-    <n v="5.9914645471079797E-3"/>
-    <n v="0.99765258215962405"/>
-  </r>
-  <r>
-    <x v="2"/>
-    <x v="0"/>
+    <n v="4.2796175336485502"/>
+    <n v="0.99756097560975598"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="1"/>
     <n v="0"/>
     <x v="4"/>
-    <n v="2.9957322735539899E-3"/>
-    <n v="0.99765258215962405"/>
-  </r>
-  <r>
-    <x v="2"/>
-    <x v="0"/>
+    <n v="2.99573227355399"/>
+    <n v="0.99756097560975598"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="1"/>
     <n v="0"/>
     <x v="5"/>
-    <n v="5.9914645471079804E-4"/>
-    <n v="0.99765258215962405"/>
-  </r>
-  <r>
-    <x v="2"/>
-    <x v="0"/>
+    <n v="1.4978661367769901"/>
+    <n v="0.99756097560975598"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="1"/>
     <n v="0"/>
     <x v="6"/>
-    <n v="2.9957322735539902E-4"/>
-    <n v="0.99765258215962405"/>
-  </r>
-  <r>
-    <x v="2"/>
-    <x v="1"/>
-    <n v="0"/>
-    <x v="0"/>
     <n v="0.29957322735539899"/>
-    <n v="0.99765258215962405"/>
-  </r>
-  <r>
-    <x v="2"/>
-    <x v="1"/>
-    <n v="0"/>
-    <x v="1"/>
-    <n v="5.9914645471079803E-2"/>
-    <n v="0.99765258215962405"/>
-  </r>
-  <r>
-    <x v="2"/>
-    <x v="1"/>
-    <n v="0"/>
-    <x v="2"/>
-    <n v="2.9957322735539901E-2"/>
-    <n v="0.99765258215962405"/>
-  </r>
-  <r>
-    <x v="2"/>
-    <x v="1"/>
-    <n v="0"/>
+    <n v="0.99756097560975598"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="0"/>
+    <x v="7"/>
+    <n v="0.14978661367769899"/>
+    <n v="0.99756097560975598"/>
+  </r>
+  <r>
     <x v="3"/>
-    <n v="5.9914645471079797E-3"/>
-    <n v="0.99765258215962405"/>
-  </r>
-  <r>
-    <x v="2"/>
-    <x v="1"/>
-    <n v="0"/>
-    <x v="4"/>
-    <n v="2.9957322735539899E-3"/>
-    <n v="0.99765258215962405"/>
-  </r>
-  <r>
-    <x v="2"/>
-    <x v="1"/>
-    <n v="0"/>
-    <x v="5"/>
-    <n v="5.9914645471079804E-4"/>
-    <n v="0.99765258215962405"/>
-  </r>
-  <r>
-    <x v="2"/>
-    <x v="1"/>
-    <n v="0"/>
-    <x v="6"/>
-    <n v="2.9957322735539902E-4"/>
-    <n v="0.99765258215962405"/>
-  </r>
-  <r>
-    <x v="3"/>
     <x v="2"/>
     <m/>
-    <x v="7"/>
+    <x v="8"/>
     <m/>
     <m/>
   </r>
@@ -818,7 +867,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{32CB7000-83E9-4F59-B65C-C7B6F8A37157}" name="PivotTable3" cacheId="18" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{32CB7000-83E9-4F59-B65C-C7B6F8A37157}" name="PivotTable3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:G10" firstHeaderRow="1" firstDataRow="3" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="6">
     <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
@@ -918,8 +967,8 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9EF27EFA-D1F2-4DCF-BBB6-95A079418BB5}" name="PivotTable4" cacheId="23" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A3:G13" firstHeaderRow="1" firstDataRow="3" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D031EEA0-56FE-4051-B358-C7672166E309}" name="PivotTable1" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:G14" firstHeaderRow="1" firstDataRow="3" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="6">
     <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
       <items count="5">
@@ -940,7 +989,7 @@
     </pivotField>
     <pivotField showAll="0"/>
     <pivotField axis="axisRow" showAll="0">
-      <items count="9">
+      <items count="10">
         <item x="0"/>
         <item x="1"/>
         <item x="2"/>
@@ -949,6 +998,7 @@
         <item x="5"/>
         <item x="6"/>
         <item x="7"/>
+        <item x="8"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -958,7 +1008,7 @@
   <rowFields count="1">
     <field x="3"/>
   </rowFields>
-  <rowItems count="8">
+  <rowItems count="9">
     <i>
       <x/>
     </i>
@@ -979,6 +1029,9 @@
     </i>
     <i>
       <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
     </i>
     <i t="grand">
       <x/>
@@ -2032,11 +2085,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C85E2ED0-A792-4A6B-8458-5916B1089B1D}">
-  <dimension ref="A1:G13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8B1158D-08EA-44CE-9A16-A7A0E87983EA}">
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2049,9 +2102,7 @@
     <col min="6" max="6" width="24.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="22.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="24" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -2100,22 +2151,22 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
-        <v>10</v>
+        <v>0.1</v>
       </c>
       <c r="B6" s="4">
-        <v>0.29957322735539899</v>
+        <v>29.957322735539901</v>
       </c>
       <c r="C6" s="4">
         <v>0.99943757030371205</v>
       </c>
       <c r="D6" s="4">
-        <v>0.29957322735539899</v>
+        <v>29.957322735539901</v>
       </c>
       <c r="E6" s="4">
         <v>0.99943757030371205</v>
       </c>
       <c r="F6" s="4">
-        <v>0.59914645471079797</v>
+        <v>59.914645471079801</v>
       </c>
       <c r="G6" s="4">
         <v>1.9988751406074241</v>
@@ -2123,22 +2174,22 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
-        <v>50</v>
+        <v>0.3</v>
       </c>
       <c r="B7" s="4">
-        <v>5.9914645471079803E-2</v>
+        <v>9.9857742451799698</v>
       </c>
       <c r="C7" s="4">
         <v>0.99943757030371205</v>
       </c>
       <c r="D7" s="4">
-        <v>5.9914645471079803E-2</v>
+        <v>9.9857742451799698</v>
       </c>
       <c r="E7" s="4">
         <v>0.99943757030371205</v>
       </c>
       <c r="F7" s="4">
-        <v>0.11982929094215961</v>
+        <v>19.97154849035994</v>
       </c>
       <c r="G7" s="4">
         <v>1.9988751406074241</v>
@@ -2146,22 +2197,22 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
-        <v>100</v>
+        <v>0.5</v>
       </c>
       <c r="B8" s="4">
-        <v>2.9957322735539901E-2</v>
+        <v>5.9914645471079799</v>
       </c>
       <c r="C8" s="4">
         <v>0.99943757030371205</v>
       </c>
       <c r="D8" s="4">
-        <v>2.9957322735539901E-2</v>
+        <v>5.9914645471079799</v>
       </c>
       <c r="E8" s="4">
         <v>0.99943757030371205</v>
       </c>
       <c r="F8" s="4">
-        <v>5.9914645471079803E-2</v>
+        <v>11.98292909421596</v>
       </c>
       <c r="G8" s="4">
         <v>1.9988751406074241</v>
@@ -2169,22 +2220,22 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
-        <v>500</v>
+        <v>0.7</v>
       </c>
       <c r="B9" s="4">
-        <v>5.9914645471079797E-3</v>
+        <v>4.2796175336485502</v>
       </c>
       <c r="C9" s="4">
         <v>0.99943757030371205</v>
       </c>
       <c r="D9" s="4">
-        <v>5.9914645471079797E-3</v>
+        <v>4.2796175336485502</v>
       </c>
       <c r="E9" s="4">
         <v>0.99943757030371205</v>
       </c>
       <c r="F9" s="4">
-        <v>1.1982929094215959E-2</v>
+        <v>8.5592350672971005</v>
       </c>
       <c r="G9" s="4">
         <v>1.9988751406074241</v>
@@ -2192,22 +2243,22 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="B10" s="4">
-        <v>2.9957322735539899E-3</v>
+        <v>2.99573227355399</v>
       </c>
       <c r="C10" s="4">
         <v>0.99943757030371205</v>
       </c>
       <c r="D10" s="4">
-        <v>2.9957322735539899E-3</v>
+        <v>2.99573227355399</v>
       </c>
       <c r="E10" s="4">
         <v>0.99943757030371205</v>
       </c>
       <c r="F10" s="4">
-        <v>5.9914645471079797E-3</v>
+        <v>5.9914645471079799</v>
       </c>
       <c r="G10" s="4">
         <v>1.9988751406074241</v>
@@ -2215,22 +2266,22 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
-        <v>5000</v>
+        <v>2</v>
       </c>
       <c r="B11" s="4">
-        <v>5.9914645471079804E-4</v>
+        <v>1.4978661367769901</v>
       </c>
       <c r="C11" s="4">
         <v>0.99943757030371205</v>
       </c>
       <c r="D11" s="4">
-        <v>5.9914645471079804E-4</v>
+        <v>1.4978661367769901</v>
       </c>
       <c r="E11" s="4">
         <v>0.99943757030371205</v>
       </c>
       <c r="F11" s="4">
-        <v>1.1982929094215961E-3</v>
+        <v>2.9957322735539802</v>
       </c>
       <c r="G11" s="4">
         <v>1.9988751406074241</v>
@@ -2238,48 +2289,71 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
-        <v>10000</v>
+        <v>10</v>
       </c>
       <c r="B12" s="4">
-        <v>2.9957322735539902E-4</v>
+        <v>0.29957322735539899</v>
       </c>
       <c r="C12" s="4">
         <v>0.99943757030371205</v>
       </c>
       <c r="D12" s="4">
-        <v>2.9957322735539902E-4</v>
+        <v>0.29957322735539899</v>
       </c>
       <c r="E12" s="4">
         <v>0.99943757030371205</v>
       </c>
       <c r="F12" s="4">
-        <v>5.9914645471079804E-4</v>
+        <v>0.59914645471079797</v>
       </c>
       <c r="G12" s="4">
         <v>1.9988751406074241</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="3">
+        <v>20</v>
+      </c>
+      <c r="B13" s="4">
+        <v>0.14978661367769899</v>
+      </c>
+      <c r="C13" s="4">
+        <v>0.99943757030343505</v>
+      </c>
+      <c r="D13" s="4">
+        <v>0.14978661367769899</v>
+      </c>
+      <c r="E13" s="4">
+        <v>0.99943757030343505</v>
+      </c>
+      <c r="F13" s="4">
+        <v>0.29957322735539799</v>
+      </c>
+      <c r="G13" s="4">
+        <v>1.9988751406068701</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="4">
-        <v>0.39933111206474686</v>
-      </c>
-      <c r="C13" s="4">
-        <v>6.9960629921259843</v>
-      </c>
-      <c r="D13" s="4">
-        <v>0.39933111206474686</v>
-      </c>
-      <c r="E13" s="4">
-        <v>6.9960629921259843</v>
-      </c>
-      <c r="F13" s="4">
-        <v>0.79866222412949373</v>
-      </c>
-      <c r="G13" s="4">
-        <v>13.992125984251969</v>
+      <c r="B14" s="4">
+        <v>55.157137312840476</v>
+      </c>
+      <c r="C14" s="4">
+        <v>7.9955005624294193</v>
+      </c>
+      <c r="D14" s="4">
+        <v>55.157137312840476</v>
+      </c>
+      <c r="E14" s="4">
+        <v>7.9955005624294193</v>
+      </c>
+      <c r="F14" s="4">
+        <v>110.31427462568095</v>
+      </c>
+      <c r="G14" s="4">
+        <v>15.991001124858839</v>
       </c>
     </row>
   </sheetData>
@@ -2289,10 +2363,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7C2440C-0365-4391-A5B0-33CFB8588B7A}">
-  <dimension ref="A1:F43"/>
+  <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16:E23"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2300,8 +2374,7 @@
     <col min="1" max="1" width="22.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -2335,10 +2408,10 @@
         <v>0</v>
       </c>
       <c r="D2">
-        <v>10</v>
+        <v>0.1</v>
       </c>
       <c r="E2">
-        <v>0.29957322735539899</v>
+        <v>29.957322735539901</v>
       </c>
       <c r="F2" t="s">
         <v>14</v>
@@ -2355,10 +2428,10 @@
         <v>0</v>
       </c>
       <c r="D3">
-        <v>50</v>
+        <v>0.3</v>
       </c>
       <c r="E3">
-        <v>5.9914645471079803E-2</v>
+        <v>9.9857742451799698</v>
       </c>
       <c r="F3" t="s">
         <v>14</v>
@@ -2375,10 +2448,10 @@
         <v>0</v>
       </c>
       <c r="D4">
-        <v>100</v>
+        <v>0.5</v>
       </c>
       <c r="E4">
-        <v>2.9957322735539901E-2</v>
+        <v>5.9914645471079799</v>
       </c>
       <c r="F4" t="s">
         <v>14</v>
@@ -2395,10 +2468,10 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>500</v>
+        <v>0.7</v>
       </c>
       <c r="E5">
-        <v>5.9914645471079797E-3</v>
+        <v>4.2796175336485502</v>
       </c>
       <c r="F5" t="s">
         <v>14</v>
@@ -2415,10 +2488,10 @@
         <v>0</v>
       </c>
       <c r="D6">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="E6">
-        <v>2.9957322735539899E-3</v>
+        <v>2.99573227355399</v>
       </c>
       <c r="F6" t="s">
         <v>14</v>
@@ -2435,10 +2508,10 @@
         <v>0</v>
       </c>
       <c r="D7">
-        <v>5000</v>
+        <v>2</v>
       </c>
       <c r="E7">
-        <v>5.9914645471079804E-4</v>
+        <v>1.4978661367769901</v>
       </c>
       <c r="F7" t="s">
         <v>14</v>
@@ -2455,10 +2528,10 @@
         <v>0</v>
       </c>
       <c r="D8">
-        <v>10000</v>
+        <v>10</v>
       </c>
       <c r="E8">
-        <v>2.9957322735539902E-4</v>
+        <v>0.29957322735539899</v>
       </c>
       <c r="F8" t="s">
         <v>14</v>
@@ -2469,16 +2542,16 @@
         <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C9">
         <v>0</v>
       </c>
       <c r="D9">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E9">
-        <v>0.29957322735539899</v>
+        <v>0.14978661367769899</v>
       </c>
       <c r="F9" t="s">
         <v>14</v>
@@ -2495,10 +2568,10 @@
         <v>0</v>
       </c>
       <c r="D10">
-        <v>50</v>
+        <v>0.1</v>
       </c>
       <c r="E10">
-        <v>5.9914645471079803E-2</v>
+        <v>29.957322735539901</v>
       </c>
       <c r="F10" t="s">
         <v>14</v>
@@ -2515,10 +2588,10 @@
         <v>0</v>
       </c>
       <c r="D11">
-        <v>100</v>
+        <v>0.3</v>
       </c>
       <c r="E11">
-        <v>2.9957322735539901E-2</v>
+        <v>9.9857742451799698</v>
       </c>
       <c r="F11" t="s">
         <v>14</v>
@@ -2535,10 +2608,10 @@
         <v>0</v>
       </c>
       <c r="D12">
-        <v>500</v>
+        <v>0.5</v>
       </c>
       <c r="E12">
-        <v>5.9914645471079797E-3</v>
+        <v>5.9914645471079799</v>
       </c>
       <c r="F12" t="s">
         <v>14</v>
@@ -2555,10 +2628,10 @@
         <v>0</v>
       </c>
       <c r="D13">
-        <v>1000</v>
+        <v>0.7</v>
       </c>
       <c r="E13">
-        <v>2.9957322735539899E-3</v>
+        <v>4.2796175336485502</v>
       </c>
       <c r="F13" t="s">
         <v>14</v>
@@ -2575,10 +2648,10 @@
         <v>0</v>
       </c>
       <c r="D14">
-        <v>5000</v>
+        <v>1</v>
       </c>
       <c r="E14">
-        <v>5.9914645471079804E-4</v>
+        <v>2.99573227355399</v>
       </c>
       <c r="F14" t="s">
         <v>14</v>
@@ -2595,10 +2668,10 @@
         <v>0</v>
       </c>
       <c r="D15">
-        <v>10000</v>
+        <v>2</v>
       </c>
       <c r="E15">
-        <v>2.9957322735539902E-4</v>
+        <v>1.4978661367769901</v>
       </c>
       <c r="F15" t="s">
         <v>14</v>
@@ -2606,10 +2679,10 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B16" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C16">
         <v>0</v>
@@ -2620,28 +2693,28 @@
       <c r="E16">
         <v>0.29957322735539899</v>
       </c>
-      <c r="F16">
-        <v>0.99943757030371205</v>
+      <c r="F16" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B17" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C17">
         <v>0</v>
       </c>
       <c r="D17">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="E17">
-        <v>5.9914645471079803E-2</v>
-      </c>
-      <c r="F17">
-        <v>0.99943757030371205</v>
+        <v>0.14978661367769899</v>
+      </c>
+      <c r="F17" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -2655,10 +2728,10 @@
         <v>0</v>
       </c>
       <c r="D18">
-        <v>100</v>
+        <v>0.1</v>
       </c>
       <c r="E18">
-        <v>2.9957322735539901E-2</v>
+        <v>29.957322735539901</v>
       </c>
       <c r="F18">
         <v>0.99943757030371205</v>
@@ -2675,10 +2748,10 @@
         <v>0</v>
       </c>
       <c r="D19">
-        <v>500</v>
+        <v>0.3</v>
       </c>
       <c r="E19">
-        <v>5.9914645471079797E-3</v>
+        <v>9.9857742451799698</v>
       </c>
       <c r="F19">
         <v>0.99943757030371205</v>
@@ -2695,10 +2768,10 @@
         <v>0</v>
       </c>
       <c r="D20">
-        <v>1000</v>
+        <v>0.5</v>
       </c>
       <c r="E20">
-        <v>2.9957322735539899E-3</v>
+        <v>5.9914645471079799</v>
       </c>
       <c r="F20">
         <v>0.99943757030371205</v>
@@ -2715,10 +2788,10 @@
         <v>0</v>
       </c>
       <c r="D21">
-        <v>5000</v>
+        <v>0.7</v>
       </c>
       <c r="E21">
-        <v>5.9914645471079804E-4</v>
+        <v>4.2796175336485502</v>
       </c>
       <c r="F21">
         <v>0.99943757030371205</v>
@@ -2735,10 +2808,10 @@
         <v>0</v>
       </c>
       <c r="D22">
-        <v>10000</v>
+        <v>1</v>
       </c>
       <c r="E22">
-        <v>2.9957322735539902E-4</v>
+        <v>2.99573227355399</v>
       </c>
       <c r="F22">
         <v>0.99943757030371205</v>
@@ -2749,16 +2822,16 @@
         <v>10</v>
       </c>
       <c r="B23" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C23">
         <v>0</v>
       </c>
       <c r="D23">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="E23">
-        <v>0.29957322735539899</v>
+        <v>1.4978661367769901</v>
       </c>
       <c r="F23">
         <v>0.99943757030371205</v>
@@ -2769,16 +2842,16 @@
         <v>10</v>
       </c>
       <c r="B24" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C24">
         <v>0</v>
       </c>
       <c r="D24">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="E24">
-        <v>5.9914645471079803E-2</v>
+        <v>0.29957322735539899</v>
       </c>
       <c r="F24">
         <v>0.99943757030371205</v>
@@ -2789,19 +2862,19 @@
         <v>10</v>
       </c>
       <c r="B25" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C25">
         <v>0</v>
       </c>
       <c r="D25">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="E25">
-        <v>2.9957322735539901E-2</v>
+        <v>0.14978661367769899</v>
       </c>
       <c r="F25">
-        <v>0.99943757030371205</v>
+        <v>0.99943757030343505</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -2815,10 +2888,10 @@
         <v>0</v>
       </c>
       <c r="D26">
-        <v>500</v>
+        <v>0.1</v>
       </c>
       <c r="E26">
-        <v>5.9914645471079797E-3</v>
+        <v>29.957322735539901</v>
       </c>
       <c r="F26">
         <v>0.99943757030371205</v>
@@ -2835,10 +2908,10 @@
         <v>0</v>
       </c>
       <c r="D27">
-        <v>1000</v>
+        <v>0.3</v>
       </c>
       <c r="E27">
-        <v>2.9957322735539899E-3</v>
+        <v>9.9857742451799698</v>
       </c>
       <c r="F27">
         <v>0.99943757030371205</v>
@@ -2855,10 +2928,10 @@
         <v>0</v>
       </c>
       <c r="D28">
-        <v>5000</v>
+        <v>0.5</v>
       </c>
       <c r="E28">
-        <v>5.9914645471079804E-4</v>
+        <v>5.9914645471079799</v>
       </c>
       <c r="F28">
         <v>0.99943757030371205</v>
@@ -2875,10 +2948,10 @@
         <v>0</v>
       </c>
       <c r="D29">
-        <v>10000</v>
+        <v>0.7</v>
       </c>
       <c r="E29">
-        <v>2.9957322735539902E-4</v>
+        <v>4.2796175336485502</v>
       </c>
       <c r="F29">
         <v>0.99943757030371205</v>
@@ -2886,82 +2959,82 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B30" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C30">
         <v>0</v>
       </c>
       <c r="D30">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="E30">
-        <v>0.29957322735539899</v>
+        <v>2.99573227355399</v>
       </c>
       <c r="F30">
-        <v>0.99765258215962405</v>
+        <v>0.99943757030371205</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B31" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C31">
         <v>0</v>
       </c>
       <c r="D31">
-        <v>50</v>
+        <v>2</v>
       </c>
       <c r="E31">
-        <v>5.9914645471079803E-2</v>
+        <v>1.4978661367769901</v>
       </c>
       <c r="F31">
-        <v>0.99765258215962405</v>
+        <v>0.99943757030371205</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B32" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C32">
         <v>0</v>
       </c>
       <c r="D32">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="E32">
-        <v>2.9957322735539901E-2</v>
+        <v>0.29957322735539899</v>
       </c>
       <c r="F32">
-        <v>0.99765258215962405</v>
+        <v>0.99943757030371205</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B33" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C33">
         <v>0</v>
       </c>
       <c r="D33">
-        <v>500</v>
+        <v>20</v>
       </c>
       <c r="E33">
-        <v>5.9914645471079797E-3</v>
+        <v>0.14978661367769899</v>
       </c>
       <c r="F33">
-        <v>0.99765258215962405</v>
+        <v>0.99943757030343505</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -2975,13 +3048,13 @@
         <v>0</v>
       </c>
       <c r="D34">
-        <v>1000</v>
+        <v>0.1</v>
       </c>
       <c r="E34">
-        <v>2.9957322735539899E-3</v>
+        <v>29.957322735539901</v>
       </c>
       <c r="F34">
-        <v>0.99765258215962405</v>
+        <v>0.99756097560975598</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -2995,13 +3068,13 @@
         <v>0</v>
       </c>
       <c r="D35">
-        <v>5000</v>
+        <v>0.3</v>
       </c>
       <c r="E35">
-        <v>5.9914645471079804E-4</v>
+        <v>9.9857742451799698</v>
       </c>
       <c r="F35">
-        <v>0.99765258215962405</v>
+        <v>0.99756097560975598</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -3015,13 +3088,13 @@
         <v>0</v>
       </c>
       <c r="D36">
-        <v>10000</v>
+        <v>0.5</v>
       </c>
       <c r="E36">
-        <v>2.9957322735539902E-4</v>
+        <v>5.9914645471079799</v>
       </c>
       <c r="F36">
-        <v>0.99765258215962405</v>
+        <v>0.99756097560975598</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -3029,19 +3102,19 @@
         <v>11</v>
       </c>
       <c r="B37" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C37">
         <v>0</v>
       </c>
       <c r="D37">
-        <v>10</v>
+        <v>0.7</v>
       </c>
       <c r="E37">
-        <v>0.29957322735539899</v>
+        <v>4.2796175336485502</v>
       </c>
       <c r="F37">
-        <v>0.99765258215962405</v>
+        <v>0.99756097560975598</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
@@ -3049,19 +3122,19 @@
         <v>11</v>
       </c>
       <c r="B38" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C38">
         <v>0</v>
       </c>
       <c r="D38">
-        <v>50</v>
+        <v>1</v>
       </c>
       <c r="E38">
-        <v>5.9914645471079803E-2</v>
+        <v>2.99573227355399</v>
       </c>
       <c r="F38">
-        <v>0.99765258215962405</v>
+        <v>0.99756097560975598</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
@@ -3069,19 +3142,19 @@
         <v>11</v>
       </c>
       <c r="B39" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C39">
         <v>0</v>
       </c>
       <c r="D39">
-        <v>100</v>
+        <v>2</v>
       </c>
       <c r="E39">
-        <v>2.9957322735539901E-2</v>
+        <v>1.4978661367769901</v>
       </c>
       <c r="F39">
-        <v>0.99765258215962405</v>
+        <v>0.99756097560975598</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
@@ -3089,19 +3162,19 @@
         <v>11</v>
       </c>
       <c r="B40" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C40">
         <v>0</v>
       </c>
       <c r="D40">
-        <v>500</v>
+        <v>10</v>
       </c>
       <c r="E40">
-        <v>5.9914645471079797E-3</v>
+        <v>0.29957322735539899</v>
       </c>
       <c r="F40">
-        <v>0.99765258215962405</v>
+        <v>0.99756097560975598</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
@@ -3109,19 +3182,19 @@
         <v>11</v>
       </c>
       <c r="B41" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C41">
         <v>0</v>
       </c>
       <c r="D41">
-        <v>1000</v>
+        <v>20</v>
       </c>
       <c r="E41">
-        <v>2.9957322735539899E-3</v>
+        <v>0.14978661367769899</v>
       </c>
       <c r="F41">
-        <v>0.99765258215962405</v>
+        <v>0.99756097560975598</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
@@ -3135,13 +3208,13 @@
         <v>0</v>
       </c>
       <c r="D42">
-        <v>5000</v>
+        <v>0.1</v>
       </c>
       <c r="E42">
-        <v>5.9914645471079804E-4</v>
+        <v>29.957322735539901</v>
       </c>
       <c r="F42">
-        <v>0.99765258215962405</v>
+        <v>0.99756097560975598</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
@@ -3155,13 +3228,133 @@
         <v>0</v>
       </c>
       <c r="D43">
-        <v>10000</v>
+        <v>0.3</v>
       </c>
       <c r="E43">
-        <v>2.9957322735539902E-4</v>
+        <v>9.9857742451799698</v>
       </c>
       <c r="F43">
-        <v>0.99765258215962405</v>
+        <v>0.99756097560975598</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>11</v>
+      </c>
+      <c r="B44" t="s">
+        <v>9</v>
+      </c>
+      <c r="C44">
+        <v>0</v>
+      </c>
+      <c r="D44">
+        <v>0.5</v>
+      </c>
+      <c r="E44">
+        <v>5.9914645471079799</v>
+      </c>
+      <c r="F44">
+        <v>0.99756097560975598</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>11</v>
+      </c>
+      <c r="B45" t="s">
+        <v>9</v>
+      </c>
+      <c r="C45">
+        <v>0</v>
+      </c>
+      <c r="D45">
+        <v>0.7</v>
+      </c>
+      <c r="E45">
+        <v>4.2796175336485502</v>
+      </c>
+      <c r="F45">
+        <v>0.99756097560975598</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>11</v>
+      </c>
+      <c r="B46" t="s">
+        <v>9</v>
+      </c>
+      <c r="C46">
+        <v>0</v>
+      </c>
+      <c r="D46">
+        <v>1</v>
+      </c>
+      <c r="E46">
+        <v>2.99573227355399</v>
+      </c>
+      <c r="F46">
+        <v>0.99756097560975598</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>11</v>
+      </c>
+      <c r="B47" t="s">
+        <v>9</v>
+      </c>
+      <c r="C47">
+        <v>0</v>
+      </c>
+      <c r="D47">
+        <v>2</v>
+      </c>
+      <c r="E47">
+        <v>1.4978661367769901</v>
+      </c>
+      <c r="F47">
+        <v>0.99756097560975598</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>11</v>
+      </c>
+      <c r="B48" t="s">
+        <v>9</v>
+      </c>
+      <c r="C48">
+        <v>0</v>
+      </c>
+      <c r="D48">
+        <v>10</v>
+      </c>
+      <c r="E48">
+        <v>0.29957322735539899</v>
+      </c>
+      <c r="F48">
+        <v>0.99756097560975598</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>11</v>
+      </c>
+      <c r="B49" t="s">
+        <v>9</v>
+      </c>
+      <c r="C49">
+        <v>0</v>
+      </c>
+      <c r="D49">
+        <v>20</v>
+      </c>
+      <c r="E49">
+        <v>0.14978661367769899</v>
+      </c>
+      <c r="F49">
+        <v>0.99756097560975598</v>
       </c>
     </row>
   </sheetData>

</xml_diff>